<commit_message>
M1 Cod code Changes updated
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -163,10 +163,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -201,13 +201,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -216,30 +210,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -268,14 +277,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -284,6 +285,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -302,7 +311,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -316,30 +332,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -360,13 +360,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -378,7 +504,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,157 +528,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,17 +584,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -648,184 +668,164 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1183,8 +1183,8 @@
   <sheetPr/>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -1334,7 +1334,7 @@
   <sheetPr/>
   <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Codes of M3 changes and Cart Page.
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A960DED-A24D-40EC-9ECC-C34A631EFDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFB6A4A-A4A8-4671-9D37-ADB1EFA42309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -242,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -295,11 +295,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -333,12 +346,19 @@
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,10 +783,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -775,43 +795,43 @@
     <col min="2" max="2" width="64.21875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -822,10 +842,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF42F157-904A-4C1C-83E9-6764862CA94E}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -834,33 +854,45 @@
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="27.6" thickBot="1">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:2" ht="27">
+      <c r="A2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
+    <row r="4" spans="1:2">
+      <c r="A4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -869,10 +901,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C97B171-CF25-42FC-A01E-B0793772DE9C}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -904,6 +936,22 @@
         <v>37</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -914,7 +962,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Pushing Code chages for M3,Login and Cart page
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFB6A4A-A4A8-4671-9D37-ADB1EFA42309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D88DD5-7A7D-4BD3-B2F0-D27BA44E915E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,7 +637,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -845,7 +845,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -887,11 +887,11 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>30</v>
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alternate Brand and Mostb Selling Product Code
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFB6A4A-A4A8-4671-9D37-ADB1EFA42309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -24,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -167,6 +161,21 @@
     <t>Sahyog Wellness Multi Function</t>
   </si>
   <si>
+    <t>Telma 40mg Tablet 30'S</t>
+  </si>
+  <si>
+    <t>Telma 40mg Tablet 30</t>
+  </si>
+  <si>
+    <t>Jusdee 400IU Drops 30ml</t>
+  </si>
+  <si>
+    <t>Kanzomin New Strawberry Flavour Granules 10gm</t>
+  </si>
+  <si>
+    <t>Keraglo Men Tablet 10'S</t>
+  </si>
+  <si>
     <t>Telmikind 40mg Tablet 10'S</t>
   </si>
   <si>
@@ -174,15 +183,6 @@
   </si>
   <si>
     <t>Korandil 5mg Tablet 10'S</t>
-  </si>
-  <si>
-    <t>Jusdee 400IU Drops 30ml</t>
-  </si>
-  <si>
-    <t>Kanzomin New Strawberry Flavour Granules 10gm</t>
-  </si>
-  <si>
-    <t>Keraglo Men Tablet 10'S</t>
   </si>
   <si>
     <t>Keppra 500mg Tablet 10'S</t>
@@ -194,14 +194,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -210,25 +228,157 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,12 +391,226 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -281,96 +645,354 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -628,373 +1250,390 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="78.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="78.4444444444444" style="8" customWidth="1"/>
+    <col min="2" max="2" width="69.4444444444444" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="15.15" spans="1:2">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="15.15" spans="1:2">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
+    <row r="3" ht="15.15" spans="1:2">
+      <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="7" t="s">
+    <row r="4" ht="15.15" spans="1:2">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="26.4">
-      <c r="A5" s="7" t="s">
+    <row r="5" ht="27.15" spans="1:2">
+      <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="7" t="s">
+    <row r="6" ht="15.15" spans="1:2">
+      <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="7" t="s">
+    <row r="7" ht="15.15" spans="1:2">
+      <c r="A7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="7" t="s">
+    <row r="8" ht="15.15" spans="1:2">
+      <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="7" t="s">
+    <row r="9" ht="15.15" spans="1:2">
+      <c r="A9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="7" t="s">
+    <row r="10" ht="15.15" spans="1:2">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="26.4">
-      <c r="A11" s="7" t="s">
+    <row r="11" ht="27.15" spans="1:2">
+      <c r="A11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="7" t="s">
+    <row r="12" ht="15.15" spans="1:2">
+      <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="10" t="s">
+    <row r="13" ht="15.15" spans="1:2">
+      <c r="A13" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="26.4">
-      <c r="A14" s="7" t="s">
+    <row r="14" ht="27.15" spans="1:2">
+      <c r="A14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="26.4">
-      <c r="A15" s="7" t="s">
+    <row r="15" ht="27.15" spans="1:2">
+      <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="7" t="s">
+    <row r="16" ht="15.15" spans="1:2">
+      <c r="A16" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="14" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="75.77734375" customWidth="1"/>
-    <col min="2" max="2" width="64.21875" customWidth="1"/>
+    <col min="1" max="1" width="75.7777777777778" customWidth="1"/>
+    <col min="2" max="2" width="64.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF42F157-904A-4C1C-83E9-6764862CA94E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="34.21875" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" ht="26.4" spans="1:2">
+      <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B2" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="27">
-      <c r="A2" s="15" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="6" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C97B171-CF25-42FC-A01E-B0793772DE9C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="23.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>35</v>
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>36</v>
+      <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>37</v>
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>41</v>
+      <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>42</v>
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA90627-010F-47C2-BD1B-8EF6C32BCBB3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="23.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>36</v>
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>41</v>
+      <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>42</v>
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cold Storage Delivery PINCODE check Code
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Otcandnonrx" sheetId="3" r:id="rId3"/>
     <sheet name="Rx" sheetId="4" r:id="rId4"/>
     <sheet name="Pastrx" sheetId="5" r:id="rId5"/>
+    <sheet name="ColdStorage" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -190,16 +191,25 @@
   <si>
     <t>Moxovas 0.3mg Tablet 10'S</t>
   </si>
+  <si>
+    <t>180001</t>
+  </si>
+  <si>
+    <t>600055</t>
+  </si>
+  <si>
+    <t>600100</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -234,8 +244,52 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -243,21 +297,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -265,15 +320,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,92 +358,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -393,25 +403,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,157 +565,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,11 +655,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -657,8 +673,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -678,6 +694,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -693,17 +718,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -722,171 +752,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -937,6 +947,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1409,7 +1420,7 @@
   <sheetPr/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1636,4 +1647,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="23.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="18.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="14.7777777777778" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="3:3">
+      <c r="C2" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3">
+      <c r="C3" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
COD 3 Processing Order Code
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="5"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Rx" sheetId="4" r:id="rId4"/>
     <sheet name="Pastrx" sheetId="5" r:id="rId5"/>
     <sheet name="ColdStorage" sheetId="6" r:id="rId6"/>
+    <sheet name="COD_Process" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -200,16 +201,31 @@
   <si>
     <t>600100</t>
   </si>
+  <si>
+    <t>Dolo 650mg Tablet 15'S</t>
+  </si>
+  <si>
+    <t>Pro360 Diabetic Nutritional Powder - Real Badam Flavour 250 gm</t>
+  </si>
+  <si>
+    <t>Pro360 Diabetic Nutritional Powder</t>
+  </si>
+  <si>
+    <t>DIGITAL THERMOMETER (AMKAY) Device 1's</t>
+  </si>
+  <si>
+    <t>DIGITAL THERMOMETER</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -244,6 +260,51 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -252,57 +313,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -319,10 +329,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -334,40 +368,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -382,6 +391,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -403,19 +419,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,163 +569,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,6 +671,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -666,15 +702,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -727,17 +754,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -755,148 +771,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1654,7 +1670,7 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1690,4 +1706,57 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="37.5555555555556" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Codes Changes for stage
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11B78E8-1F01-4487-B2E8-1F8C992C88E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
     <sheet name="COD_Check" sheetId="2" r:id="rId2"/>
     <sheet name="Otcandnonrx" sheetId="3" r:id="rId3"/>
-    <sheet name="Rx" sheetId="4" r:id="rId4"/>
-    <sheet name="Pastrx" sheetId="5" r:id="rId5"/>
-    <sheet name="ColdStorage" sheetId="6" r:id="rId6"/>
-    <sheet name="COD_Process" sheetId="7" r:id="rId7"/>
+    <sheet name="OCT&amp;NonRX_Stage" sheetId="8" r:id="rId4"/>
+    <sheet name="Rx" sheetId="4" r:id="rId5"/>
+    <sheet name="Pastrx" sheetId="5" r:id="rId6"/>
+    <sheet name="ColdStorage" sheetId="6" r:id="rId7"/>
+    <sheet name="COD_Process" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -220,14 +227,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,152 +260,8 @@
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -417,194 +274,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -670,253 +341,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -965,61 +394,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1277,26 +662,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="78.4444444444444" style="8" customWidth="1"/>
-    <col min="2" max="2" width="69.4444444444444" style="8" customWidth="1"/>
+    <col min="1" max="1" width="78.44140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="69.44140625" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.15" spans="1:2">
+    <row r="1" spans="1:2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1304,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="15.15" spans="1:2">
+    <row r="2" spans="1:2">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1312,7 +697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" ht="15.15" spans="1:2">
+    <row r="3" spans="1:2">
       <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
@@ -1320,7 +705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="15.15" spans="1:2">
+    <row r="4" spans="1:2">
       <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
@@ -1328,7 +713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="27.15" spans="1:2">
+    <row r="5" spans="1:2" ht="26.4">
       <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
@@ -1336,7 +721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="15.15" spans="1:2">
+    <row r="6" spans="1:2">
       <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
@@ -1344,7 +729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="15.15" spans="1:2">
+    <row r="7" spans="1:2">
       <c r="A7" s="13" t="s">
         <v>11</v>
       </c>
@@ -1352,7 +737,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" ht="15.15" spans="1:2">
+    <row r="8" spans="1:2">
       <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
@@ -1360,7 +745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" ht="15.15" spans="1:2">
+    <row r="9" spans="1:2">
       <c r="A9" s="13" t="s">
         <v>14</v>
       </c>
@@ -1368,7 +753,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" ht="15.15" spans="1:2">
+    <row r="10" spans="1:2">
       <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
@@ -1376,7 +761,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" ht="27.15" spans="1:2">
+    <row r="11" spans="1:2" ht="26.4">
       <c r="A11" s="13" t="s">
         <v>16</v>
       </c>
@@ -1384,7 +769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" ht="15.15" spans="1:2">
+    <row r="12" spans="1:2">
       <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
@@ -1392,7 +777,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" ht="15.15" spans="1:2">
+    <row r="13" spans="1:2">
       <c r="A13" s="16" t="s">
         <v>19</v>
       </c>
@@ -1400,7 +785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" ht="27.15" spans="1:2">
+    <row r="14" spans="1:2" ht="26.4">
       <c r="A14" s="13" t="s">
         <v>21</v>
       </c>
@@ -1408,7 +793,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" ht="27.15" spans="1:2">
+    <row r="15" spans="1:2" ht="26.4">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -1416,7 +801,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" ht="15.15" spans="1:2">
+    <row r="16" spans="1:2">
       <c r="A16" s="13" t="s">
         <v>25</v>
       </c>
@@ -1425,25 +810,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="75.7777777777778" customWidth="1"/>
-    <col min="2" max="2" width="64.2222222222222" customWidth="1"/>
+    <col min="1" max="1" width="75.77734375" customWidth="1"/>
+    <col min="2" max="2" width="64.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1496,23 +879,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="34.21875" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1523,7 +904,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" ht="26.4" spans="1:2">
+    <row r="2" spans="1:2" ht="27">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
@@ -1557,22 +938,71 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048D418C-264F-4EF6-B3F4-9DE0BEF25755}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="34.21875" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="27">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="23.3333333333333" customWidth="1"/>
+    <col min="1" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1617,22 +1047,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="23.5555555555556" customWidth="1"/>
+    <col min="1" max="2" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1661,24 +1089,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="18.8888888888889" customWidth="1"/>
-    <col min="3" max="3" width="14.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1692,34 +1118,32 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="3:3">
+    <row r="2" spans="1:3">
       <c r="C2" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="3:3">
+    <row r="3" spans="1:3">
       <c r="C3" s="18" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="37.5555555555556" customWidth="1"/>
+    <col min="1" max="1" width="37.5546875" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1757,6 +1181,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
COD 3 Processing Order Stage Code Changes
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11B78E8-1F01-4487-B2E8-1F8C992C88E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -27,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -176,6 +170,23 @@
     <t>Telma 40mg Tablet 30</t>
   </si>
   <si>
+    <r>
+      <t>Nestle Peptamen Peptide Based Diet Powder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF151B39"/>
+        <rFont val="Lato"/>
+        <charset val="134"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>INLIFE Whey Protein Powder Chocolate Flavor 2 kg</t>
+  </si>
+  <si>
     <t>Jusdee 400IU Drops 30ml</t>
   </si>
   <si>
@@ -227,14 +238,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -243,25 +272,163 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF151B39"/>
+      <name val="Lato"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,8 +441,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -341,49 +694,291 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -394,17 +989,61 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -662,26 +1301,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="78.44140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="78.4444444444444" style="8" customWidth="1"/>
+    <col min="2" max="2" width="69.4444444444444" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" ht="15.15" spans="1:2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -689,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" ht="15.15" spans="1:2">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -697,7 +1336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" ht="15.15" spans="1:2">
       <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
@@ -705,7 +1344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" ht="15.15" spans="1:2">
       <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
@@ -713,7 +1352,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="26.4">
+    <row r="5" ht="27.15" spans="1:2">
       <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
@@ -721,7 +1360,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" ht="15.15" spans="1:2">
       <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
@@ -729,7 +1368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" ht="15.15" spans="1:2">
       <c r="A7" s="13" t="s">
         <v>11</v>
       </c>
@@ -737,7 +1376,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" ht="15.15" spans="1:2">
       <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
@@ -745,7 +1384,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" ht="15.15" spans="1:2">
       <c r="A9" s="13" t="s">
         <v>14</v>
       </c>
@@ -753,7 +1392,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" ht="15.15" spans="1:2">
       <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
@@ -761,7 +1400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="26.4">
+    <row r="11" ht="27.15" spans="1:2">
       <c r="A11" s="13" t="s">
         <v>16</v>
       </c>
@@ -769,7 +1408,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" ht="15.15" spans="1:2">
       <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
@@ -777,7 +1416,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" ht="15.15" spans="1:2">
       <c r="A13" s="16" t="s">
         <v>19</v>
       </c>
@@ -785,7 +1424,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="26.4">
+    <row r="14" ht="27.15" spans="1:2">
       <c r="A14" s="13" t="s">
         <v>21</v>
       </c>
@@ -793,7 +1432,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="26.4">
+    <row r="15" ht="27.15" spans="1:2">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -801,7 +1440,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" ht="15.15" spans="1:2">
       <c r="A16" s="13" t="s">
         <v>25</v>
       </c>
@@ -810,23 +1449,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="75.77734375" customWidth="1"/>
-    <col min="2" max="2" width="64.21875" customWidth="1"/>
+    <col min="1" max="1" width="75.7777777777778" customWidth="1"/>
+    <col min="2" max="2" width="64.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -877,234 +1518,292 @@
         <v>36</v>
       </c>
     </row>
+    <row r="8" ht="18.6" spans="1:2">
+      <c r="A8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="34.21875" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="27">
-      <c r="A2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>38</v>
+      <c r="A1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" ht="26.4" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>39</v>
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048D418C-264F-4EF6-B3F4-9DE0BEF25755}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="34.21875" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27">
-      <c r="A1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>38</v>
+    <row r="1" ht="26.4" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="23.33203125" customWidth="1"/>
+    <col min="1" max="2" width="23.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="23.5546875" customWidth="1"/>
+    <col min="1" max="2" width="23.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="18.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="14.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1115,41 +1814,43 @@
         <v>0</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="3:3">
       <c r="C2" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3">
       <c r="C3" s="18" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" customWidth="1"/>
+    <col min="1" max="1" width="37.5555555555556" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
@@ -1157,23 +1858,23 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -1181,5 +1882,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code changes for Linked account and for Cartpage
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB3AAB5-2A92-4A43-B7A2-4F8B42543A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -234,18 +240,15 @@
   <si>
     <t>DIGITAL THERMOMETER</t>
   </si>
+  <si>
+    <t>Folvite Tablet 45'S</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,157 +281,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="15"/>
       <color rgb="FF151B39"/>
       <name val="Lato"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,194 +300,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -694,253 +367,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -989,61 +420,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1301,26 +688,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="78.4444444444444" style="8" customWidth="1"/>
-    <col min="2" max="2" width="69.4444444444444" style="8" customWidth="1"/>
+    <col min="1" max="1" width="78.44140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="69.44140625" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.15" spans="1:2">
+    <row r="1" spans="1:2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1328,7 +715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="15.15" spans="1:2">
+    <row r="2" spans="1:2">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1336,7 +723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" ht="15.15" spans="1:2">
+    <row r="3" spans="1:2">
       <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
@@ -1344,7 +731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="15.15" spans="1:2">
+    <row r="4" spans="1:2">
       <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
@@ -1352,7 +739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="27.15" spans="1:2">
+    <row r="5" spans="1:2" ht="26.4">
       <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
@@ -1360,7 +747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="15.15" spans="1:2">
+    <row r="6" spans="1:2">
       <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
@@ -1368,7 +755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="15.15" spans="1:2">
+    <row r="7" spans="1:2">
       <c r="A7" s="13" t="s">
         <v>11</v>
       </c>
@@ -1376,7 +763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" ht="15.15" spans="1:2">
+    <row r="8" spans="1:2">
       <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
@@ -1384,7 +771,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" ht="15.15" spans="1:2">
+    <row r="9" spans="1:2">
       <c r="A9" s="13" t="s">
         <v>14</v>
       </c>
@@ -1392,7 +779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" ht="15.15" spans="1:2">
+    <row r="10" spans="1:2">
       <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
@@ -1400,7 +787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" ht="27.15" spans="1:2">
+    <row r="11" spans="1:2" ht="26.4">
       <c r="A11" s="13" t="s">
         <v>16</v>
       </c>
@@ -1408,7 +795,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" ht="15.15" spans="1:2">
+    <row r="12" spans="1:2">
       <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
@@ -1416,7 +803,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" ht="15.15" spans="1:2">
+    <row r="13" spans="1:2">
       <c r="A13" s="16" t="s">
         <v>19</v>
       </c>
@@ -1424,7 +811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" ht="27.15" spans="1:2">
+    <row r="14" spans="1:2" ht="26.4">
       <c r="A14" s="13" t="s">
         <v>21</v>
       </c>
@@ -1432,7 +819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" ht="27.15" spans="1:2">
+    <row r="15" spans="1:2" ht="26.4">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -1440,7 +827,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" ht="15.15" spans="1:2">
+    <row r="16" spans="1:2">
       <c r="A16" s="13" t="s">
         <v>25</v>
       </c>
@@ -1449,25 +836,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="75.7777777777778" customWidth="1"/>
-    <col min="2" max="2" width="64.2222222222222" customWidth="1"/>
+    <col min="1" max="1" width="75.77734375" customWidth="1"/>
+    <col min="2" max="2" width="64.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1518,7 +903,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" ht="18.6" spans="1:2">
+    <row r="8" spans="1:2" ht="19.2">
       <c r="A8" s="7" t="s">
         <v>37</v>
       </c>
@@ -1568,23 +953,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="34.21875" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1595,7 +978,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" ht="26.4" spans="1:2">
+    <row r="2" spans="1:2" ht="27">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1605,10 +988,10 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1629,26 +1012,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="34.21875" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.4" spans="1:2">
+    <row r="1" spans="1:2" ht="27">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
@@ -1682,22 +1063,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="23.3333333333333" customWidth="1"/>
+    <col min="1" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1742,22 +1121,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="23.5555555555556" customWidth="1"/>
+    <col min="1" max="2" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1786,24 +1163,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="18.8888888888889" customWidth="1"/>
-    <col min="3" max="3" width="14.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1817,34 +1192,32 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="3:3">
+    <row r="2" spans="1:3">
       <c r="C2" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="3:3">
+    <row r="3" spans="1:3">
       <c r="C3" s="18" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="37.5555555555556" customWidth="1"/>
+    <col min="1" max="1" width="37.5546875" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1882,6 +1255,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Order Successpage Code Updated
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB3AAB5-2A92-4A43-B7A2-4F8B42543A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA0A3BD-31FE-4774-A9F5-87ED7E5BE7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t>Kanzomin New Strawberry Flavour Granules 10gm</t>
-  </si>
-  <si>
-    <t>Keraglo Men Tablet 10'S</t>
   </si>
   <si>
     <t>Telmikind 40mg Tablet 10'S</t>
@@ -960,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -988,10 +985,10 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1017,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1029,35 +1026,43 @@
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="27">
+      <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>28</v>
+      <c r="A3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1081,42 +1086,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1139,26 +1144,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1189,17 +1194,17 @@
         <v>0</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="C2" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="C3" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1228,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
@@ -1231,23 +1236,23 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
         <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
POM and M3 Flow code
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA0A3BD-31FE-4774-A9F5-87ED7E5BE7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A9861D-40CC-4645-9907-A2BF56C2851D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5712" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -957,9 +957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
@@ -1016,9 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>

</xml_diff>

<commit_message>
After dry Code updated for EHR,Cart page,M3 flow,My order,Order success page, Previous consultation, XLSX,
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CF7B00-22F3-47BA-B986-13B8D8CFDF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -250,23 +256,27 @@
   <si>
     <t>Horlicks</t>
   </si>
+  <si>
+    <t>Patanjali Dant Kanti Tooth Paste - Natural (200 gm + 100 gm)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -294,157 +304,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="15"/>
       <color rgb="FF151B39"/>
       <name val="Lato"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,194 +323,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -710,356 +390,71 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1317,26 +712,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="78.4444444444444" style="8" customWidth="1"/>
-    <col min="2" max="2" width="69.4444444444444" style="8" customWidth="1"/>
+    <col min="1" max="1" width="78.44140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="69.44140625" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.15" spans="1:2">
+    <row r="1" spans="1:2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1344,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="15.15" spans="1:2">
+    <row r="2" spans="1:2">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1352,7 +747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" ht="15.15" spans="1:2">
+    <row r="3" spans="1:2">
       <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
@@ -1360,7 +755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="15.15" spans="1:2">
+    <row r="4" spans="1:2">
       <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
@@ -1368,7 +763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="27.15" spans="1:2">
+    <row r="5" spans="1:2" ht="26.4">
       <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
@@ -1376,7 +771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="15.15" spans="1:2">
+    <row r="6" spans="1:2">
       <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
@@ -1384,7 +779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="15.15" spans="1:2">
+    <row r="7" spans="1:2">
       <c r="A7" s="13" t="s">
         <v>11</v>
       </c>
@@ -1392,7 +787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" ht="15.15" spans="1:2">
+    <row r="8" spans="1:2">
       <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
@@ -1400,7 +795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" ht="15.15" spans="1:2">
+    <row r="9" spans="1:2">
       <c r="A9" s="13" t="s">
         <v>14</v>
       </c>
@@ -1408,7 +803,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" ht="15.15" spans="1:2">
+    <row r="10" spans="1:2">
       <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
@@ -1416,7 +811,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" ht="27.15" spans="1:2">
+    <row r="11" spans="1:2" ht="26.4">
       <c r="A11" s="13" t="s">
         <v>16</v>
       </c>
@@ -1424,7 +819,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" ht="15.15" spans="1:2">
+    <row r="12" spans="1:2">
       <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
@@ -1432,7 +827,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" ht="15.15" spans="1:2">
+    <row r="13" spans="1:2">
       <c r="A13" s="16" t="s">
         <v>19</v>
       </c>
@@ -1440,7 +835,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" ht="27.15" spans="1:2">
+    <row r="14" spans="1:2" ht="26.4">
       <c r="A14" s="13" t="s">
         <v>21</v>
       </c>
@@ -1448,7 +843,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" ht="27.15" spans="1:2">
+    <row r="15" spans="1:2" ht="26.4">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -1456,7 +851,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" ht="15.15" spans="1:2">
+    <row r="16" spans="1:2">
       <c r="A16" s="13" t="s">
         <v>25</v>
       </c>
@@ -1465,25 +860,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="75.7777777777778" customWidth="1"/>
-    <col min="2" max="2" width="64.2222222222222" customWidth="1"/>
+    <col min="1" max="1" width="75.77734375" customWidth="1"/>
+    <col min="2" max="2" width="64.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1534,7 +927,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" ht="18.6" spans="1:2">
+    <row r="8" spans="1:2" ht="19.2">
       <c r="A8" s="7" t="s">
         <v>37</v>
       </c>
@@ -1584,23 +977,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1611,7 +1002,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" ht="26.4" spans="1:2">
+    <row r="2" spans="1:2" ht="27">
       <c r="A2" s="4" t="s">
         <v>40</v>
       </c>
@@ -1643,25 +1034,32 @@
         <v>30</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="34.21875" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1672,7 +1070,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" ht="26.4" spans="1:2">
+    <row r="2" spans="1:2" ht="27">
       <c r="A2" s="4" t="s">
         <v>40</v>
       </c>
@@ -1704,24 +1102,30 @@
         <v>30</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="23.3333333333333" customWidth="1"/>
+    <col min="1" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1766,22 +1170,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="23.5555555555556" customWidth="1"/>
+    <col min="1" max="2" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1810,24 +1212,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="18.8888888888889" customWidth="1"/>
-    <col min="3" max="3" width="14.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1841,34 +1241,32 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="3:3">
+    <row r="2" spans="1:3">
       <c r="C2" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="3:3">
+    <row r="3" spans="1:3">
       <c r="C3" s="18" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="37.5555555555556" customWidth="1"/>
+    <col min="1" max="1" width="37.5546875" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1906,20 +1304,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1938,6 +1334,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
M2 Flow  Code Update
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CF7B00-22F3-47BA-B986-13B8D8CFDF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="23040" windowHeight="9335" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -22,13 +16,14 @@
     <sheet name="ColdStorage" sheetId="6" r:id="rId7"/>
     <sheet name="COD_Process" sheetId="7" r:id="rId8"/>
     <sheet name="AndPDP" sheetId="9" r:id="rId9"/>
+    <sheet name="AndM2" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -209,6 +204,9 @@
     <t>Folvite Tablet 45'S</t>
   </si>
   <si>
+    <t>Patanjali Dant Kanti Tooth Paste - Natural (200 gm + 100 gm)</t>
+  </si>
+  <si>
     <t>Telmikind 40mg Tablet 10'S</t>
   </si>
   <si>
@@ -257,26 +255,25 @@
     <t>Horlicks</t>
   </si>
   <si>
-    <t>Patanjali Dant Kanti Tooth Paste - Natural (200 gm + 100 gm)</t>
+    <t>Telma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -299,9 +296,160 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="15"/>
@@ -310,7 +458,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +471,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -390,49 +724,292 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -442,19 +1019,62 @@
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -712,286 +1332,312 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="78.44140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" style="8" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="8"/>
+    <col min="1" max="1" width="78.4444444444444" style="9" customWidth="1"/>
+    <col min="2" max="2" width="69.4444444444444" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="9" t="s">
+    <row r="1" ht="15.15" spans="1:2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="9" t="s">
+    <row r="2" ht="15.15" spans="1:2">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="11" t="s">
+    <row r="3" ht="15.15" spans="1:2">
+      <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="13" t="s">
+    <row r="4" ht="15.15" spans="1:2">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="26.4">
-      <c r="A5" s="13" t="s">
+    <row r="5" ht="27.15" spans="1:2">
+      <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="13" t="s">
+    <row r="6" ht="15.15" spans="1:2">
+      <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="13" t="s">
+    <row r="7" ht="15.15" spans="1:2">
+      <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="13" t="s">
+    <row r="8" ht="15.15" spans="1:2">
+      <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="13" t="s">
+    <row r="9" ht="15.15" spans="1:2">
+      <c r="A9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="13" t="s">
+    <row r="10" ht="15.15" spans="1:2">
+      <c r="A10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="26.4">
-      <c r="A11" s="13" t="s">
+    <row r="11" ht="27.15" spans="1:2">
+      <c r="A11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="13" t="s">
+    <row r="12" ht="15.15" spans="1:2">
+      <c r="A12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="16" t="s">
+    <row r="13" ht="15.15" spans="1:2">
+      <c r="A13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="26.4">
-      <c r="A14" s="13" t="s">
+    <row r="14" ht="27.15" spans="1:2">
+      <c r="A14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="26.4">
-      <c r="A15" s="13" t="s">
+    <row r="15" ht="27.15" spans="1:2">
+      <c r="A15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="13" t="s">
+    <row r="16" ht="15.15" spans="1:2">
+      <c r="A16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="15" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="75.77734375" customWidth="1"/>
-    <col min="2" max="2" width="64.21875" customWidth="1"/>
+    <col min="1" max="1" width="75.7777777777778" customWidth="1"/>
+    <col min="2" max="2" width="64.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.2">
-      <c r="A8" s="7" t="s">
+    <row r="8" ht="18.6" spans="1:2">
+      <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="51.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="1" max="1" width="51.1111111111111" customWidth="1"/>
+    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1002,7 +1648,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="27">
+    <row r="2" ht="26.4" spans="1:2">
       <c r="A2" s="4" t="s">
         <v>40</v>
       </c>
@@ -1036,30 +1682,32 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>58</v>
+        <v>42</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="34.21875" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1070,7 +1718,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="27">
+    <row r="2" ht="26.4" spans="1:2">
       <c r="A2" s="4" t="s">
         <v>40</v>
       </c>
@@ -1104,130 +1752,136 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="23.33203125" customWidth="1"/>
+    <col min="1" max="2" width="23.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="23.5546875" customWidth="1"/>
+    <col min="1" max="2" width="23.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="18.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="14.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1237,42 +1891,44 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="C2" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="C3" s="18" t="s">
+    <row r="2" spans="3:3">
+      <c r="C2" s="19" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3">
+      <c r="C3" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" customWidth="1"/>
+    <col min="1" max="1" width="37.5555555555556" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
@@ -1280,23 +1936,23 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -1304,35 +1960,38 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
backend And miste framework
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -1,29 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\Automation\Test Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7224D2-0ED3-4BB5-A105-42661674EB84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
     <sheet name="COD_Check" sheetId="2" r:id="rId2"/>
     <sheet name="Otcandnonrx" sheetId="3" r:id="rId3"/>
-    <sheet name="OCT&amp;NonRX_Stage" sheetId="8" r:id="rId4"/>
-    <sheet name="Rx" sheetId="4" r:id="rId5"/>
+    <sheet name="Rx" sheetId="4" r:id="rId4"/>
+    <sheet name="OCT&amp;NonRX_Stage" sheetId="8" r:id="rId5"/>
     <sheet name="Pastrx" sheetId="5" r:id="rId6"/>
     <sheet name="ColdStorage" sheetId="6" r:id="rId7"/>
     <sheet name="COD_Process" sheetId="7" r:id="rId8"/>
     <sheet name="AndPDP" sheetId="9" r:id="rId9"/>
     <sheet name="AndM2" sheetId="10" r:id="rId10"/>
+    <sheet name="orderIds" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -257,18 +264,18 @@
   <si>
     <t>Telma</t>
   </si>
+  <si>
+    <t>16341194999000204W</t>
+  </si>
+  <si>
+    <t>16341199249000212W</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="26">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,157 +315,19 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="15"/>
       <color rgb="FF151B39"/>
       <name val="Lato"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF151B39"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,194 +340,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -724,253 +407,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1019,62 +460,27 @@
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1332,26 +738,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="78.4444444444444" style="9" customWidth="1"/>
-    <col min="2" max="2" width="69.4444444444444" style="9" customWidth="1"/>
+    <col min="1" max="1" width="78.44140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="69.44140625" style="9" customWidth="1"/>
     <col min="3" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.15" spans="1:2">
+    <row r="1" spans="1:2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1359,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="15.15" spans="1:2">
+    <row r="2" spans="1:2">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -1367,7 +773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" ht="15.15" spans="1:2">
+    <row r="3" spans="1:2">
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
@@ -1375,7 +781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="15.15" spans="1:2">
+    <row r="4" spans="1:2">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
@@ -1383,7 +789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="27.15" spans="1:2">
+    <row r="5" spans="1:2" ht="26.4">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -1391,7 +797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="15.15" spans="1:2">
+    <row r="6" spans="1:2">
       <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
@@ -1399,7 +805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="15.15" spans="1:2">
+    <row r="7" spans="1:2">
       <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
@@ -1407,7 +813,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" ht="15.15" spans="1:2">
+    <row r="8" spans="1:2">
       <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
@@ -1415,7 +821,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" ht="15.15" spans="1:2">
+    <row r="9" spans="1:2">
       <c r="A9" s="14" t="s">
         <v>14</v>
       </c>
@@ -1423,7 +829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" ht="15.15" spans="1:2">
+    <row r="10" spans="1:2">
       <c r="A10" s="14" t="s">
         <v>15</v>
       </c>
@@ -1431,7 +837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" ht="27.15" spans="1:2">
+    <row r="11" spans="1:2" ht="26.4">
       <c r="A11" s="14" t="s">
         <v>16</v>
       </c>
@@ -1439,7 +845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" ht="15.15" spans="1:2">
+    <row r="12" spans="1:2">
       <c r="A12" s="14" t="s">
         <v>18</v>
       </c>
@@ -1447,7 +853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" ht="15.15" spans="1:2">
+    <row r="13" spans="1:2">
       <c r="A13" s="17" t="s">
         <v>19</v>
       </c>
@@ -1455,7 +861,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" ht="27.15" spans="1:2">
+    <row r="14" spans="1:2" ht="26.4">
       <c r="A14" s="14" t="s">
         <v>21</v>
       </c>
@@ -1463,7 +869,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" ht="27.15" spans="1:2">
+    <row r="15" spans="1:2" ht="26.4">
       <c r="A15" s="14" t="s">
         <v>23</v>
       </c>
@@ -1471,7 +877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" ht="15.15" spans="1:2">
+    <row r="16" spans="1:2">
       <c r="A16" s="14" t="s">
         <v>25</v>
       </c>
@@ -1480,22 +886,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1504,23 +908,51 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2D9BFB-E38E-4119-9C15-3F83D4FAD543}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" style="21" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15">
+      <c r="A2" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="75.7777777777778" customWidth="1"/>
-    <col min="2" max="2" width="64.2222222222222" customWidth="1"/>
+    <col min="1" max="1" width="75.77734375" customWidth="1"/>
+    <col min="2" max="2" width="64.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1571,7 +1003,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" ht="18.6" spans="1:2">
+    <row r="8" spans="1:2" ht="19.2">
       <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
@@ -1621,23 +1053,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="51.1111111111111" customWidth="1"/>
-    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="51.109375" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1648,7 +1078,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" ht="26.4" spans="1:2">
+    <row r="2" spans="1:2" ht="27">
       <c r="A2" s="4" t="s">
         <v>40</v>
       </c>
@@ -1690,24 +1120,80 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="2" width="23.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="34.21875" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1718,7 +1204,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" ht="26.4" spans="1:2">
+    <row r="2" spans="1:2" ht="27">
       <c r="A2" s="4" t="s">
         <v>40</v>
       </c>
@@ -1760,82 +1246,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="2" width="23.3333333333333" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="23.5555555555556" customWidth="1"/>
+    <col min="1" max="2" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1864,24 +1288,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="18.8888888888889" customWidth="1"/>
-    <col min="3" max="3" width="14.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1895,34 +1317,32 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="3:3">
+    <row r="2" spans="1:3">
       <c r="C2" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="3:3">
+    <row r="3" spans="1:3">
       <c r="C3" s="19" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="37.5555555555556" customWidth="1"/>
+    <col min="1" max="1" width="37.5546875" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1960,20 +1380,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1992,6 +1410,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Website Stage ColdStorage update
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="5" activeTab="11"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -224,6 +224,9 @@
     <t>Moxovas 0.3mg Tablet 10'S</t>
   </si>
   <si>
+    <t>Stpase 1500000IU Injection 10ml</t>
+  </si>
+  <si>
     <t>180001</t>
   </si>
   <si>
@@ -231,6 +234,9 @@
   </si>
   <si>
     <t>600100</t>
+  </si>
+  <si>
+    <t>cscs</t>
   </si>
   <si>
     <t>Dolo 650mg Tablet 15'S</t>
@@ -274,10 +280,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -316,20 +322,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -340,6 +332,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -348,6 +362,90 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -356,83 +454,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -441,21 +462,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -483,25 +489,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,25 +651,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -543,102 +663,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -646,24 +670,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,32 +741,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -780,11 +765,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -794,6 +785,32 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -821,162 +838,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1518,7 +1524,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1544,12 +1550,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1564,7 +1570,7 @@
   <sheetPr/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1595,7 +1601,7 @@
         <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1991,13 +1997,13 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="23.2190476190476" customWidth="1"/>
     <col min="2" max="2" width="18.8857142857143" customWidth="1"/>
@@ -2006,23 +2012,28 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="3:3">
       <c r="C2" s="22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="3:3">
       <c r="C3" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2048,7 +2059,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
@@ -2056,23 +2067,23 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -2097,17 +2108,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WebSite Live Code Update
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="5" activeTab="6"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -194,6 +194,9 @@
     </r>
   </si>
   <si>
+    <t>Proquest Whey Protein Concentrate - Milk Chocolate Flavour 2 Kg</t>
+  </si>
+  <si>
     <t>INLIFE Whey Protein Powder Chocolate Flavor 2 kg</t>
   </si>
   <si>
@@ -280,9 +283,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
@@ -322,6 +325,43 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -332,15 +372,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -354,9 +434,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -369,50 +449,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -431,43 +471,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="15"/>
       <color rgb="FF151B39"/>
       <name val="Lato"/>
@@ -489,187 +492,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -741,11 +744,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -761,6 +785,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -791,6 +824,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -799,190 +841,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1524,7 +1527,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1550,12 +1553,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1582,26 +1585,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1622,10 +1625,10 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1640,7 +1643,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1710,7 +1713,7 @@
         <v>38</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1768,26 +1771,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" ht="25.5" spans="1:2">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1808,10 +1811,10 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1837,42 +1840,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1898,26 +1901,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" ht="25.5" spans="1:2">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1938,10 +1941,10 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1966,26 +1969,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2000,7 +2003,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
@@ -2012,28 +2015,28 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="3:3">
       <c r="C2" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="3:3">
       <c r="C3" s="22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2059,7 +2062,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
@@ -2067,23 +2070,23 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -2108,17 +2111,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Android POM,Covid Assesment,EHR and Order successpage
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F588A70-5F16-4A89-BF1F-A1699746CA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="2856" yWindow="2856" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -281,14 +287,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="26">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,157 +327,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="15"/>
       <color rgb="FF151B39"/>
       <name val="Lato"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,194 +346,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -743,253 +413,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1048,61 +476,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1360,26 +744,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="78.4380952380952" style="12" customWidth="1"/>
-    <col min="2" max="2" width="69.4380952380952" style="12" customWidth="1"/>
+    <col min="1" max="1" width="78.44140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="69.44140625" style="12" customWidth="1"/>
     <col min="3" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:2">
+    <row r="1" spans="1:2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1387,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:2">
+    <row r="2" spans="1:2">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -1395,7 +779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="1:2">
+    <row r="3" spans="1:2">
       <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
@@ -1403,7 +787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="1:2">
+    <row r="4" spans="1:2">
       <c r="A4" s="17" t="s">
         <v>5</v>
       </c>
@@ -1411,7 +795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="26.25" spans="1:2">
+    <row r="5" spans="1:2" ht="26.4">
       <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
@@ -1419,7 +803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="1:2">
+    <row r="6" spans="1:2">
       <c r="A6" s="17" t="s">
         <v>9</v>
       </c>
@@ -1427,7 +811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="15.75" spans="1:2">
+    <row r="7" spans="1:2">
       <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
@@ -1435,7 +819,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="1:2">
+    <row r="8" spans="1:2">
       <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
@@ -1443,7 +827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" ht="15.75" spans="1:2">
+    <row r="9" spans="1:2">
       <c r="A9" s="17" t="s">
         <v>14</v>
       </c>
@@ -1451,7 +835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" ht="15.75" spans="1:2">
+    <row r="10" spans="1:2">
       <c r="A10" s="17" t="s">
         <v>15</v>
       </c>
@@ -1459,7 +843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" ht="26.25" spans="1:2">
+    <row r="11" spans="1:2" ht="26.4">
       <c r="A11" s="17" t="s">
         <v>16</v>
       </c>
@@ -1467,7 +851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" ht="15.75" spans="1:2">
+    <row r="12" spans="1:2">
       <c r="A12" s="17" t="s">
         <v>18</v>
       </c>
@@ -1475,7 +859,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" ht="15.75" spans="1:2">
+    <row r="13" spans="1:2">
       <c r="A13" s="20" t="s">
         <v>19</v>
       </c>
@@ -1483,7 +867,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" ht="26.25" spans="1:2">
+    <row r="14" spans="1:2" ht="26.4">
       <c r="A14" s="17" t="s">
         <v>21</v>
       </c>
@@ -1491,7 +875,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" ht="26.25" spans="1:2">
+    <row r="15" spans="1:2" ht="26.4">
       <c r="A15" s="17" t="s">
         <v>23</v>
       </c>
@@ -1499,7 +883,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" ht="15.75" spans="1:2">
+    <row r="16" spans="1:2">
       <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
@@ -1508,22 +892,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1532,23 +914,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.2190476190476" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88571428571429" style="1"/>
+    <col min="1" max="1" width="25.21875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1564,23 +944,21 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="52.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="52.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1633,23 +1011,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="75.7809523809524" customWidth="1"/>
-    <col min="2" max="2" width="64.2190476190476" customWidth="1"/>
+    <col min="1" max="1" width="75.77734375" customWidth="1"/>
+    <col min="2" max="2" width="64.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1700,7 +1076,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" ht="18.75" spans="1:2">
+    <row r="8" spans="1:2" ht="19.2">
       <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
@@ -1750,23 +1126,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="51.1047619047619" customWidth="1"/>
-    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="51.109375" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1777,20 +1151,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" ht="25.5" spans="1:2">
+    <row r="2" spans="1:2">
       <c r="A2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="27">
+      <c r="A3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B3" s="8" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1819,23 +1193,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="23.3333333333333" customWidth="1"/>
+    <col min="1" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1880,23 +1252,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.2190476190476" customWidth="1"/>
-    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="34.21875" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1907,7 +1277,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" ht="25.5" spans="1:2">
+    <row r="2" spans="1:2" ht="27">
       <c r="A2" s="7" t="s">
         <v>41</v>
       </c>
@@ -1949,22 +1319,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="23.552380952381" customWidth="1"/>
+    <col min="1" max="2" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1993,24 +1361,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.2190476190476" customWidth="1"/>
-    <col min="2" max="2" width="18.8857142857143" customWidth="1"/>
-    <col min="3" max="3" width="14.7809523809524" customWidth="1"/>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2024,39 +1390,37 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="3:3">
+    <row r="2" spans="1:3">
       <c r="C2" s="22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="3:3">
+    <row r="3" spans="1:3">
       <c r="C3" s="22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="37.552380952381" customWidth="1"/>
+    <col min="1" max="1" width="37.5546875" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2094,20 +1458,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -2126,6 +1488,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cod Processing and M1 cod Code update
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F588A70-5F16-4A89-BF1F-A1699746CA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2856" yWindow="2856" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -153,7 +147,7 @@
     <t xml:space="preserve">Horlicks Health Drink Powder Classic Malt </t>
   </si>
   <si>
-    <t>Dolo 650mg Tablet 15</t>
+    <t>Dolo 500mg</t>
   </si>
   <si>
     <t>Gemer 2mg Tablet 10'S</t>
@@ -209,10 +203,13 @@
     <t>Jusdee 400IU Drops 30ml</t>
   </si>
   <si>
+    <t>Folvite Tablet 45'S</t>
+  </si>
+  <si>
     <t>Kanzomin New Strawberry Flavour Granules 10gm</t>
   </si>
   <si>
-    <t>Folvite Tablet 45'S</t>
+    <t>Dolo 650mg Tablet 15</t>
   </si>
   <si>
     <t>Patanjali Dant Kanti Tooth Paste - Natural (200 gm + 100 gm)</t>
@@ -248,19 +245,19 @@
     <t>cscs</t>
   </si>
   <si>
+    <t>Pro360 Diabetic Nutritional Powder - Real Badam Flavour 250 gm</t>
+  </si>
+  <si>
+    <t>Pro360 Diabetic Nutritional Powder</t>
+  </si>
+  <si>
+    <t>DIGITAL THERMOMETER (AMKAY) Device 1's</t>
+  </si>
+  <si>
+    <t>DIGITAL THERMOMETER</t>
+  </si>
+  <si>
     <t>Dolo 650mg Tablet 15'S</t>
-  </si>
-  <si>
-    <t>Pro360 Diabetic Nutritional Powder - Real Badam Flavour 250 gm</t>
-  </si>
-  <si>
-    <t>Pro360 Diabetic Nutritional Powder</t>
-  </si>
-  <si>
-    <t>DIGITAL THERMOMETER (AMKAY) Device 1's</t>
-  </si>
-  <si>
-    <t>DIGITAL THERMOMETER</t>
   </si>
   <si>
     <t>Gemer</t>
@@ -287,8 +284,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,13 +330,157 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="15"/>
       <color rgb="FF151B39"/>
       <name val="Lato"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,8 +493,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -413,11 +746,253 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -476,17 +1051,61 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -744,26 +1363,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="78.44140625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="78.4380952380952" style="12" customWidth="1"/>
+    <col min="2" max="2" width="69.4380952380952" style="12" customWidth="1"/>
     <col min="3" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" ht="15.75" spans="1:2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -771,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" ht="15.75" spans="1:2">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -779,7 +1398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" ht="15.75" spans="1:2">
       <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
@@ -787,7 +1406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" ht="15.75" spans="1:2">
       <c r="A4" s="17" t="s">
         <v>5</v>
       </c>
@@ -795,7 +1414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="26.4">
+    <row r="5" ht="26.25" spans="1:2">
       <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
@@ -803,7 +1422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" ht="15.75" spans="1:2">
       <c r="A6" s="17" t="s">
         <v>9</v>
       </c>
@@ -811,7 +1430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" ht="15.75" spans="1:2">
       <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
@@ -819,7 +1438,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" ht="15.75" spans="1:2">
       <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
@@ -827,7 +1446,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" ht="15.75" spans="1:2">
       <c r="A9" s="17" t="s">
         <v>14</v>
       </c>
@@ -835,7 +1454,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" ht="15.75" spans="1:2">
       <c r="A10" s="17" t="s">
         <v>15</v>
       </c>
@@ -843,7 +1462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="26.4">
+    <row r="11" ht="26.25" spans="1:2">
       <c r="A11" s="17" t="s">
         <v>16</v>
       </c>
@@ -851,7 +1470,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" ht="15.75" spans="1:2">
       <c r="A12" s="17" t="s">
         <v>18</v>
       </c>
@@ -859,7 +1478,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" ht="15.75" spans="1:2">
       <c r="A13" s="20" t="s">
         <v>19</v>
       </c>
@@ -867,7 +1486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="26.4">
+    <row r="14" ht="26.25" spans="1:2">
       <c r="A14" s="17" t="s">
         <v>21</v>
       </c>
@@ -875,7 +1494,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="26.4">
+    <row r="15" ht="26.25" spans="1:2">
       <c r="A15" s="17" t="s">
         <v>23</v>
       </c>
@@ -883,7 +1502,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" ht="15.75" spans="1:2">
       <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
@@ -892,73 +1511,79 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="25.21875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="25.2190476190476" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88571428571429" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="52.5546875" customWidth="1"/>
+    <col min="2" max="2" width="52.552380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -971,26 +1596,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1003,29 +1628,31 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="75.77734375" customWidth="1"/>
-    <col min="2" max="2" width="64.21875" customWidth="1"/>
+    <col min="1" max="1" width="75.7809523809524" customWidth="1"/>
+    <col min="2" max="2" width="64.2190476190476" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1076,7 +1703,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.2">
+    <row r="8" ht="18.75" spans="1:2">
       <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
@@ -1126,21 +1753,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="51.109375" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="1" max="1" width="51.1047619047619" customWidth="1"/>
+    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1153,26 +1782,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" ht="25.5" spans="1:2">
+      <c r="A3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B3" s="8" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="27">
-      <c r="A3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1185,88 +1814,92 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="23.33203125" customWidth="1"/>
+    <col min="1" max="2" width="23.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="34.21875" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.2190476190476" customWidth="1"/>
+    <col min="2" max="2" width="32.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1277,28 +1910,28 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="27">
+    <row r="2" ht="25.5" spans="1:2">
       <c r="A2" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1311,122 +1944,128 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="23.5546875" customWidth="1"/>
+    <col min="1" max="2" width="23.552380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.2190476190476" customWidth="1"/>
+    <col min="2" max="2" width="18.8857142857143" customWidth="1"/>
+    <col min="3" max="3" width="14.7809523809524" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="3:3">
       <c r="C2" s="22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3">
       <c r="C3" s="22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" customWidth="1"/>
+    <col min="1" max="1" width="37.552380952381" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
@@ -1450,43 +2089,46 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="2"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
We b issues fixed
</commit_message>
<xml_diff>
--- a/Test Data/SMSTEST.xlsx
+++ b/Test Data/SMSTEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F588A70-5F16-4A89-BF1F-A1699746CA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382BA0E3-E443-49C7-BE25-14B59598CD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2856" yWindow="2856" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TakeAction" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="68">
   <si>
     <t>Boostrix Injection</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>Folvite Tablet 45</t>
+  </si>
+  <si>
+    <t>2mg Tablet 10'S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dolo 650mg Tablet 15 Gemer </t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1140,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1169,18 +1175,18 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="9" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2">

</xml_diff>